<commit_message>
test view product passed
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/test_data_ebay.xlsx
+++ b/com.ebay/src/test/resources/test_data_ebay.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.ebay/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47C20AF-B979-8745-ACCE-20DA8C6226F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADA964B-F392-F943-978F-48AD99E74AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="1" xr2:uid="{D8090BBB-351B-C349-AE43-996F6E7696D5}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="2" xr2:uid="{D8090BBB-351B-C349-AE43-996F6E7696D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
     <sheet name="Search" sheetId="2" r:id="rId2"/>
+    <sheet name="ViewProduct" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -52,6 +53,21 @@
   </si>
   <si>
     <t>15032</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>apple watch series 7</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Apple Watch Series 7</t>
   </si>
 </sst>
 </file>
@@ -457,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81D5A97-BDBC-9E41-A1F1-60E8BF7D1CDF}">
   <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -481,4 +497,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6994902-2F11-D64D-915F-3226A23497EA}">
+  <dimension ref="A2:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" style="3" customWidth="1"/>
+    <col min="2" max="5" width="10.83203125" style="3"/>
+    <col min="6" max="6" width="25.5" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test shop for dslrs passed
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/test_data_ebay.xlsx
+++ b/com.ebay/src/test/resources/test_data_ebay.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.ebay/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADA964B-F392-F943-978F-48AD99E74AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9C7719-EB12-A64F-8FB9-07CB04EDC122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="2" xr2:uid="{D8090BBB-351B-C349-AE43-996F6E7696D5}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="3" xr2:uid="{D8090BBB-351B-C349-AE43-996F6E7696D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
     <sheet name="Search" sheetId="2" r:id="rId2"/>
     <sheet name="ViewProduct" sheetId="3" r:id="rId3"/>
+    <sheet name="ShopForDSLRs" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -68,6 +69,9 @@
   </si>
   <si>
     <t>Apple Watch Series 7</t>
+  </si>
+  <si>
+    <t>Canon Digital SLR Cameras between $350.00 and $750.00</t>
   </si>
 </sst>
 </file>
@@ -503,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6994902-2F11-D64D-915F-3226A23497EA}">
   <dimension ref="A2:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -538,4 +542,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E55F43F-C343-0446-A6F2-3A54A83BE73F}">
+  <dimension ref="A2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="64" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case shop for cars passed
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/test_data_ebay.xlsx
+++ b/com.ebay/src/test/resources/test_data_ebay.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.ebay/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9C7719-EB12-A64F-8FB9-07CB04EDC122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CE0BCE-E1F9-064E-9F99-2E10EE3C8A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="3" xr2:uid="{D8090BBB-351B-C349-AE43-996F6E7696D5}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="4" xr2:uid="{D8090BBB-351B-C349-AE43-996F6E7696D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
     <sheet name="Search" sheetId="2" r:id="rId2"/>
     <sheet name="ViewProduct" sheetId="3" r:id="rId3"/>
     <sheet name="ShopForDSLRs" sheetId="4" r:id="rId4"/>
+    <sheet name="ShopForChargers" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -72,6 +73,18 @@
   </si>
   <si>
     <t>Canon Digital SLR Cameras between $350.00 and $750.00</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Dodge</t>
+  </si>
+  <si>
+    <t>Charger</t>
+  </si>
+  <si>
+    <t>Dodge Charger</t>
   </si>
 </sst>
 </file>
@@ -548,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E55F43F-C343-0446-A6F2-3A54A83BE73F}">
   <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -573,4 +586,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27EEB39-8336-DC42-A245-B29246C32140}">
+  <dimension ref="A2:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="16.5" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test shop for art passed
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/test_data_ebay.xlsx
+++ b/com.ebay/src/test/resources/test_data_ebay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.ebay/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CE0BCE-E1F9-064E-9F99-2E10EE3C8A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABA11A0-0A6E-4240-896E-A5A4EDE7A5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="4" xr2:uid="{D8090BBB-351B-C349-AE43-996F6E7696D5}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="5" xr2:uid="{D8090BBB-351B-C349-AE43-996F6E7696D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ViewProduct" sheetId="3" r:id="rId3"/>
     <sheet name="ShopForDSLRs" sheetId="4" r:id="rId4"/>
     <sheet name="ShopForChargers" sheetId="5" r:id="rId5"/>
+    <sheet name="ShopForPaintings" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -85,6 +86,12 @@
   </si>
   <si>
     <t>Dodge Charger</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Watercolor Art Paintings</t>
   </si>
 </sst>
 </file>
@@ -592,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27EEB39-8336-DC42-A245-B29246C32140}">
   <dimension ref="A2:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -620,4 +627,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2030A44C-98A5-6C43-8190-4F12D211159B}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="29.1640625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case shop for rugs passed
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/test_data_ebay.xlsx
+++ b/com.ebay/src/test/resources/test_data_ebay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.ebay/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABA11A0-0A6E-4240-896E-A5A4EDE7A5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C20EF0-9082-EE4F-93B7-3A57279D3836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="5" xr2:uid="{D8090BBB-351B-C349-AE43-996F6E7696D5}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="6" xr2:uid="{D8090BBB-351B-C349-AE43-996F6E7696D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="ShopForDSLRs" sheetId="4" r:id="rId4"/>
     <sheet name="ShopForChargers" sheetId="5" r:id="rId5"/>
     <sheet name="ShopForPaintings" sheetId="6" r:id="rId6"/>
+    <sheet name="ShopForRugs" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
@@ -92,6 +93,12 @@
   </si>
   <si>
     <t>Watercolor Art Paintings</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Traditional Area Rugs</t>
   </si>
 </sst>
 </file>
@@ -633,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2030A44C-98A5-6C43-8190-4F12D211159B}">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -655,4 +662,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E659B9BB-8BF3-824E-A43A-77BE4D97C05E}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="26.33203125" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>